<commit_message>
docs: Update project schedule and related image
Updated cronograma.xlsx and its corresponding cronograma.png image to reflect the latest project timeline and milestones.
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\LojaSocial-IPCA\relatorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C908361C-D06B-4392-8996-D457A3D599BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52120964-CD7C-4C12-BA9B-39FEFE02D046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
     <t xml:space="preserve">Entrega 1: </t>
   </si>
@@ -296,15 +296,8 @@
  '25</t>
   </si>
   <si>
-    <t>2ª Entrega / apresentação</t>
-  </si>
-  <si>
     <t>dez
  '25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-</t>
   </si>
   <si>
     <t>3ª Entrega / apresentação</t>
@@ -406,19 +399,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Reunião para discussão dos requisitos </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF666666"/>
-        <rFont val="Calibri, sans-serif"/>
-      </rPr>
-      <t>(11:00h-13:00h)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Inicio da elaboração do relatório </t>
     </r>
     <r>
@@ -483,13 +463,28 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Inicio do Sprint 1
+Reunião para discussão dos requisitos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF666666"/>
+        <rFont val="Calibri, sans-serif"/>
+      </rPr>
+      <t>(11:00h-13:00h)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
         <color rgb="FF666666"/>
         <rFont val="Calibri, sans-serif"/>
       </rPr>
-      <t>Finalização da primeira entrega</t>
+      <t>Fim de Sprint 1
+Finalização da primeira entrega</t>
     </r>
     <r>
       <rPr>
@@ -500,12 +495,57 @@
       <t xml:space="preserve"> (14:00h-16:00h)</t>
     </r>
   </si>
+  <si>
+    <t>Inicio da Sprint 2</t>
+  </si>
+  <si>
+    <t>Fim de Sprint 2</t>
+  </si>
+  <si>
+    <t>Inicio do Sprint 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri, sans-serif"/>
+      </rPr>
+      <t xml:space="preserve">Fim do Sprint 3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2ª Entrega / apresentação</t>
+    </r>
+  </si>
+  <si>
+    <t>Fim do Sprint 4</t>
+  </si>
+  <si>
+    <t>Inicio do Sprint 4</t>
+  </si>
+  <si>
+    <t>Inicio do Sprint 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fim do Sprint 5
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +662,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -685,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -758,13 +810,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -784,13 +851,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,7 +860,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -861,6 +920,24 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="2" builtinId="8"/>
@@ -1199,14 +1276,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6BE823-DED3-4D53-A2A4-88602A1B888D}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="48" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="48" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
     <col min="14" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1243,678 +1320,690 @@
       <c r="B3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="13" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="13" t="s">
+      <c r="L3" s="53"/>
+      <c r="M3" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="13" t="s">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="14"/>
-    </row>
-    <row r="4" spans="1:23" ht="42" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="P3" s="53"/>
+    </row>
+    <row r="4" spans="1:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="14">
         <v>14</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="17">
+      <c r="D4" s="15"/>
+      <c r="E4" s="14">
         <v>15</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="17">
+      <c r="F4" s="16"/>
+      <c r="G4" s="14">
         <v>16</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="17">
+      <c r="H4" s="17"/>
+      <c r="I4" s="14">
         <v>17</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="14">
         <v>18</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="14">
         <v>19</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="17">
+      <c r="O4" s="14">
         <v>20</v>
       </c>
-      <c r="P4" s="18"/>
-    </row>
-    <row r="5" spans="1:23" s="44" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="37">
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="33">
         <v>2</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="34">
         <v>21</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="38">
+      <c r="D5" s="35"/>
+      <c r="E5" s="34">
         <v>22</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="34">
         <v>23</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="38">
+      <c r="H5" s="37"/>
+      <c r="I5" s="34">
         <v>24</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="38">
+      <c r="J5" s="38"/>
+      <c r="K5" s="34">
         <v>25</v>
       </c>
-      <c r="L5" s="43"/>
-      <c r="M5" s="38">
+      <c r="L5" s="39"/>
+      <c r="M5" s="34">
         <v>26</v>
       </c>
-      <c r="N5" s="45" t="s">
+      <c r="N5" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" s="34">
+        <v>27</v>
+      </c>
+      <c r="P5" s="35"/>
+    </row>
+    <row r="6" spans="1:23" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="13">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>28</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="14">
+        <v>29</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="14">
+        <v>30</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="14">
+        <v>2</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="14">
+        <v>3</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="14">
+        <v>4</v>
+      </c>
+      <c r="P6" s="15"/>
+    </row>
+    <row r="7" spans="1:23" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="13">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14">
+        <v>6</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="14">
+        <v>7</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="14">
+        <v>8</v>
+      </c>
+      <c r="K7" s="14">
+        <v>9</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="14">
+        <v>10</v>
+      </c>
+      <c r="N7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="38">
+      <c r="O7" s="14">
+        <v>11</v>
+      </c>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:23" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="13">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14">
+        <v>12</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="14">
+        <v>13</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="14">
+        <v>14</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="14">
+        <v>15</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="14">
+        <v>16</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="14">
+        <v>17</v>
+      </c>
+      <c r="N8" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" s="14">
+        <v>18</v>
+      </c>
+      <c r="P8" s="15"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="13">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14">
+        <v>19</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14">
+        <v>20</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="14">
+        <v>21</v>
+      </c>
+      <c r="I9" s="14">
+        <v>22</v>
+      </c>
+      <c r="J9" s="21"/>
+      <c r="K9" s="14">
+        <v>23</v>
+      </c>
+      <c r="L9" s="21"/>
+      <c r="M9" s="14">
+        <v>24</v>
+      </c>
+      <c r="N9" s="21"/>
+      <c r="O9" s="14">
+        <v>25</v>
+      </c>
+      <c r="P9" s="15"/>
+      <c r="W9" s="7"/>
+    </row>
+    <row r="10" spans="1:23" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="13">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14">
+        <v>26</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14">
         <v>27</v>
       </c>
-      <c r="P5" s="39"/>
-    </row>
-    <row r="6" spans="1:23" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="16">
+      <c r="F10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="14">
+        <v>28</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="14">
+        <v>29</v>
+      </c>
+      <c r="K10" s="14">
+        <v>30</v>
+      </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="14">
+        <v>31</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="O10" s="14">
+        <v>1</v>
+      </c>
+      <c r="P10" s="15"/>
+    </row>
+    <row r="11" spans="1:23" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="13">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14">
         <v>3</v>
       </c>
-      <c r="C6" s="17">
+      <c r="F11" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="14">
+        <v>4</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="14">
+        <v>5</v>
+      </c>
+      <c r="J11" s="18"/>
+      <c r="K11" s="14">
+        <v>6</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="14">
+        <v>7</v>
+      </c>
+      <c r="N11" s="17"/>
+      <c r="O11" s="14">
+        <v>8</v>
+      </c>
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:23" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="13">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14">
+        <v>9</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="14">
+        <v>10</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="14">
+        <v>11</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="14">
+        <v>12</v>
+      </c>
+      <c r="J12" s="23"/>
+      <c r="K12" s="14">
+        <v>13</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="14">
+        <v>14</v>
+      </c>
+      <c r="N12" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="O12" s="14">
+        <v>15</v>
+      </c>
+      <c r="P12" s="15"/>
+    </row>
+    <row r="13" spans="1:23" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="14">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="14">
+        <v>17</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="14">
+        <v>18</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="14">
+        <v>19</v>
+      </c>
+      <c r="K13" s="14">
+        <v>20</v>
+      </c>
+      <c r="L13" s="17"/>
+      <c r="M13" s="14">
+        <v>21</v>
+      </c>
+      <c r="N13" s="17"/>
+      <c r="O13" s="14">
+        <v>22</v>
+      </c>
+      <c r="P13" s="15"/>
+    </row>
+    <row r="14" spans="1:23" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="13">
+        <v>13</v>
+      </c>
+      <c r="C14" s="14">
+        <v>23</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="14">
+        <v>24</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="14">
+        <v>25</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="14">
+        <v>26</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="14">
+        <v>27</v>
+      </c>
+      <c r="L14" s="19"/>
+      <c r="M14" s="14">
         <v>28</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="17">
+      <c r="N14" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" s="14">
         <v>29</v>
       </c>
-      <c r="F6" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="17">
+      <c r="P14" s="15"/>
+    </row>
+    <row r="15" spans="1:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="13">
+        <v>14</v>
+      </c>
+      <c r="C15" s="14">
         <v>30</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="17">
+      <c r="D15" s="15"/>
+      <c r="E15" s="14">
         <v>1</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="17">
+      <c r="F15" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="14">
         <v>2</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="17">
+      <c r="H15" s="17"/>
+      <c r="I15" s="14">
         <v>3</v>
       </c>
-      <c r="N6" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="O6" s="17">
+      <c r="K15" s="14">
         <v>4</v>
       </c>
-      <c r="P6" s="18"/>
-    </row>
-    <row r="7" spans="1:23" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="16">
+      <c r="L15" s="17"/>
+      <c r="M15" s="14">
+        <v>5</v>
+      </c>
+      <c r="N15" s="17"/>
+      <c r="O15" s="14">
         <v>6</v>
       </c>
-      <c r="C7" s="17">
+      <c r="P15" s="15"/>
+    </row>
+    <row r="16" spans="1:23" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="13">
+        <v>15</v>
+      </c>
+      <c r="C16" s="14">
+        <v>7</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14">
+        <v>8</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="14">
+        <v>9</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="14">
+        <v>10</v>
+      </c>
+      <c r="J16" s="18"/>
+      <c r="K16" s="14">
+        <v>11</v>
+      </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="14">
+        <v>12</v>
+      </c>
+      <c r="N16" s="42"/>
+      <c r="O16" s="14">
+        <v>13</v>
+      </c>
+      <c r="P16" s="15"/>
+    </row>
+    <row r="17" spans="1:16" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="13">
+        <v>16</v>
+      </c>
+      <c r="C17" s="14">
+        <v>14</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="14">
+        <v>15</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="14">
+        <v>16</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="14">
+        <v>17</v>
+      </c>
+      <c r="J17" s="19"/>
+      <c r="K17" s="14">
+        <v>18</v>
+      </c>
+      <c r="M17" s="14">
+        <v>19</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="O17" s="14">
+        <v>20</v>
+      </c>
+      <c r="P17" s="15"/>
+    </row>
+    <row r="18" spans="1:16" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="13">
+        <v>17</v>
+      </c>
+      <c r="C18" s="14">
+        <v>21</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14">
+        <v>22</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="14">
+        <v>23</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="14">
+        <v>24</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="14">
+        <v>25</v>
+      </c>
+      <c r="L18" s="25"/>
+      <c r="M18" s="14">
+        <v>26</v>
+      </c>
+      <c r="N18" s="21"/>
+      <c r="O18" s="14">
+        <v>27</v>
+      </c>
+      <c r="P18" s="15"/>
+    </row>
+    <row r="19" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="51"/>
+      <c r="B19" s="13">
+        <v>18</v>
+      </c>
+      <c r="C19" s="14">
+        <v>28</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14">
+        <v>29</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="14">
+        <v>30</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="14">
+        <v>31</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="14">
+        <v>1</v>
+      </c>
+      <c r="L19" s="21"/>
+      <c r="M19" s="14">
+        <v>2</v>
+      </c>
+      <c r="N19" s="21"/>
+      <c r="O19" s="14">
+        <v>3</v>
+      </c>
+      <c r="P19" s="15"/>
+    </row>
+    <row r="20" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="13">
+        <v>14</v>
+      </c>
+      <c r="C20" s="14">
+        <v>4</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="14">
         <v>5</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="17">
+      <c r="F20" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="14">
         <v>6</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="17">
+      <c r="H20" s="17"/>
+      <c r="I20" s="14">
         <v>7</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="17">
+      <c r="K20" s="14">
         <v>8</v>
       </c>
-      <c r="K7" s="17">
+      <c r="M20" s="14">
         <v>9</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="17">
+      <c r="N20" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="O20" s="14">
         <v>10</v>
       </c>
-      <c r="N7" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="O7" s="17">
+      <c r="P20" s="15"/>
+    </row>
+    <row r="21" spans="1:16" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="13">
+        <v>15</v>
+      </c>
+      <c r="C21" s="14">
         <v>11</v>
       </c>
-      <c r="P7" s="18"/>
-    </row>
-    <row r="8" spans="1:23" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="16">
-        <v>7</v>
-      </c>
-      <c r="C8" s="17">
+      <c r="D21" s="15"/>
+      <c r="E21" s="46">
         <v>12</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17">
+      <c r="F21" s="49"/>
+      <c r="G21" s="47">
         <v>13</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="17">
+      <c r="H21" s="22"/>
+      <c r="I21" s="14">
         <v>14</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="17">
-        <v>15</v>
-      </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="17">
-        <v>16</v>
-      </c>
-      <c r="L8" s="20"/>
-      <c r="M8" s="17">
-        <v>17</v>
-      </c>
-      <c r="N8" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="O8" s="17">
-        <v>18</v>
-      </c>
-      <c r="P8" s="18"/>
-    </row>
-    <row r="9" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="16">
-        <v>8</v>
-      </c>
-      <c r="C9" s="17">
-        <v>19</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17">
-        <v>20</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="17">
-        <v>21</v>
-      </c>
-      <c r="I9" s="17">
-        <v>22</v>
-      </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="17">
-        <v>23</v>
-      </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="17">
-        <v>24</v>
-      </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="17">
-        <v>25</v>
-      </c>
-      <c r="P9" s="18"/>
-      <c r="W9" s="7"/>
-    </row>
-    <row r="10" spans="1:23" ht="111" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="16">
-        <v>9</v>
-      </c>
-      <c r="C10" s="17">
-        <v>26</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="17">
-        <v>27</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="17">
-        <v>28</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="17">
-        <v>29</v>
-      </c>
-      <c r="K10" s="17">
-        <v>30</v>
-      </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="17">
-        <v>31</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="O10" s="17">
-        <v>1</v>
-      </c>
-      <c r="P10" s="18"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="16">
-        <v>10</v>
-      </c>
-      <c r="C11" s="17">
-        <v>2</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17">
-        <v>3</v>
-      </c>
-      <c r="G11" s="17">
-        <v>4</v>
-      </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="17">
-        <v>5</v>
-      </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="17">
-        <v>6</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="17">
-        <v>7</v>
-      </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="17">
-        <v>8</v>
-      </c>
-      <c r="P11" s="18"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="16">
-        <v>11</v>
-      </c>
-      <c r="C12" s="17">
-        <v>9</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17">
-        <v>10</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="17">
-        <v>11</v>
-      </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="17">
-        <v>12</v>
-      </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="17">
-        <v>13</v>
-      </c>
-      <c r="L12" s="27"/>
-      <c r="M12" s="17">
-        <v>14</v>
-      </c>
-      <c r="N12" s="20"/>
-      <c r="O12" s="17">
-        <v>15</v>
-      </c>
-      <c r="P12" s="18"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="16">
-        <v>12</v>
-      </c>
-      <c r="C13" s="17">
-        <v>16</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="17">
-        <v>17</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="17">
-        <v>18</v>
-      </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="17">
-        <v>19</v>
-      </c>
-      <c r="K13" s="17">
-        <v>20</v>
-      </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="17">
-        <v>21</v>
-      </c>
-      <c r="N13" s="20"/>
-      <c r="O13" s="17">
-        <v>22</v>
-      </c>
-      <c r="P13" s="18"/>
-    </row>
-    <row r="14" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="16">
-        <v>13</v>
-      </c>
-      <c r="C14" s="17">
-        <v>23</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="17">
-        <v>24</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="17">
-        <v>25</v>
-      </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="17">
-        <v>26</v>
-      </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="17">
-        <v>27</v>
-      </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="17">
-        <v>28</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="O14" s="17">
-        <v>29</v>
-      </c>
-      <c r="P14" s="18"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="16">
-        <v>14</v>
-      </c>
-      <c r="C15" s="17">
-        <v>30</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17">
-        <v>1</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="17">
-        <v>2</v>
-      </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="17">
-        <v>3</v>
-      </c>
-      <c r="K15" s="17">
-        <v>4</v>
-      </c>
-      <c r="L15" s="20"/>
-      <c r="M15" s="17">
-        <v>5</v>
-      </c>
-      <c r="N15" s="20"/>
-      <c r="O15" s="17">
-        <v>6</v>
-      </c>
-      <c r="P15" s="18"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="17">
-        <v>7</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17">
-        <v>8</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="17">
-        <v>9</v>
-      </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="17">
-        <v>10</v>
-      </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="17">
-        <v>11</v>
-      </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="17">
-        <v>12</v>
-      </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="17">
-        <v>13</v>
-      </c>
-      <c r="P16" s="18"/>
-    </row>
-    <row r="17" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="16">
-        <v>16</v>
-      </c>
-      <c r="C17" s="17">
-        <v>14</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="17">
-        <v>15</v>
-      </c>
-      <c r="G17" s="17">
-        <v>16</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="17">
-        <v>17</v>
-      </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="17">
-        <v>18</v>
-      </c>
-      <c r="M17" s="17">
-        <v>19</v>
-      </c>
-      <c r="N17" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="O17" s="17">
-        <v>20</v>
-      </c>
-      <c r="P17" s="18"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="16">
-        <v>17</v>
-      </c>
-      <c r="C18" s="17">
-        <v>21</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="17">
-        <v>22</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="17">
-        <v>23</v>
-      </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="17">
-        <v>24</v>
-      </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="17">
-        <v>25</v>
-      </c>
-      <c r="L18" s="29"/>
-      <c r="M18" s="17">
-        <v>26</v>
-      </c>
-      <c r="N18" s="25"/>
-      <c r="O18" s="17">
-        <v>27</v>
-      </c>
-      <c r="P18" s="18"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="16">
-        <v>18</v>
-      </c>
-      <c r="C19" s="17">
-        <v>28</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="17">
-        <v>29</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="17">
-        <v>30</v>
-      </c>
-      <c r="H19" s="29"/>
-      <c r="I19" s="17">
-        <v>31</v>
-      </c>
-      <c r="J19" s="25"/>
-      <c r="K19" s="17">
-        <v>1</v>
-      </c>
-      <c r="L19" s="25"/>
-      <c r="M19" s="17">
-        <v>2</v>
-      </c>
-      <c r="N19" s="25"/>
-      <c r="O19" s="17">
-        <v>3</v>
-      </c>
-      <c r="P19" s="18"/>
-    </row>
-    <row r="20" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="J21" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="16">
-        <v>14</v>
-      </c>
-      <c r="C20" s="17">
-        <v>4</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="17">
-        <v>5</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="17">
-        <v>6</v>
-      </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="17">
-        <v>7</v>
-      </c>
-      <c r="K20" s="17">
-        <v>8</v>
-      </c>
-      <c r="M20" s="17">
-        <v>9</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O20" s="17">
-        <v>10</v>
-      </c>
-      <c r="P20" s="18"/>
-    </row>
-    <row r="21" spans="1:16" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="16">
-        <v>15</v>
-      </c>
-      <c r="C21" s="17">
-        <v>11</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="17">
-        <v>12</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="17">
-        <v>13</v>
-      </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="17">
-        <v>14</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="18"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="15"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
+      <c r="A22" s="26"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
@@ -1923,7 +2012,7 @@
       <c r="P22" s="11"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
+      <c r="A23" s="26"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
       <c r="L23" s="11"/>
@@ -1933,16 +2022,16 @@
       <c r="P23" s="11"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
-      <c r="H24" s="31" t="s">
-        <v>64</v>
+      <c r="H24" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -1952,16 +2041,16 @@
       <c r="P24" s="11"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="30"/>
-      <c r="B25" s="32" t="s">
-        <v>65</v>
+      <c r="A25" s="26"/>
+      <c r="B25" s="28" t="s">
+        <v>63</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
@@ -1971,16 +2060,16 @@
       <c r="P25" s="11"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="30"/>
-      <c r="B26" s="32" t="s">
-        <v>68</v>
+      <c r="A26" s="26"/>
+      <c r="B26" s="28" t="s">
+        <v>66</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
@@ -1990,117 +2079,117 @@
       <c r="P26" s="11"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="33"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="11"/>
       <c r="H27" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="33"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="11"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="11"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="33"/>
-      <c r="B30" s="32"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="11"/>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="29"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="11"/>
+      <c r="H31" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="29"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="11"/>
+      <c r="H32" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="33"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="11"/>
-      <c r="H31" s="35" t="s">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="29"/>
+      <c r="H33" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="33"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="11"/>
-      <c r="H32" s="36">
-        <v>0.1</v>
-      </c>
-      <c r="I32" s="1" t="s">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="29"/>
+      <c r="H34" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="33"/>
-      <c r="H33" s="36">
-        <v>0.25</v>
-      </c>
-      <c r="I33" s="1" t="s">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="29"/>
+      <c r="H35" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
-      <c r="H34" s="36">
-        <v>0.25</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="33"/>
-      <c r="H35" s="36">
-        <v>0.4</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="H36" s="36"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="H37" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
-      <c r="H38" s="36"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="H38" s="32"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="33"/>
-      <c r="H39" s="36"/>
+      <c r="A39" s="29"/>
+      <c r="H39" s="32"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="33"/>
+      <c r="A40" s="29"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="33"/>
+      <c r="A41" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2109,13 +2198,13 @@
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F9" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{40893C99-8889-497D-B662-6514644C9EFC}"/>
@@ -2124,6 +2213,7 @@
     <hyperlink ref="N20" location="Entregas!A43" display="4ª Entrega / apresentação" xr:uid="{76AE8F67-9041-4958-924B-3E1DF0422B8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2131,8 +2221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBF2D1-CADC-44D3-8848-D81CAA5E17FC}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2197,7 +2287,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1"/>
     </row>
@@ -2215,7 +2305,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" s="1"/>
     </row>
@@ -2228,32 +2318,32 @@
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
docs: Update project schedule and BPMN diagram files
Updated Cronograma.xlsx and Diagrama_BPMN.vpp in the docs directory to reflect recent changes in the project timeline and process modeling.
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\LojaSocial-IPCA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52120964-CD7C-4C12-BA9B-39FEFE02D046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44088F9B-92F4-4867-8AB1-FDA894EDCB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t xml:space="preserve">Entrega 1: </t>
   </si>
@@ -63,18 +63,6 @@
     <t>Documento de Requisitos</t>
   </si>
   <si>
-    <t>:: Casos de uso </t>
-  </si>
-  <si>
-    <t>:: Diagrama de modelo de dados (ER) </t>
-  </si>
-  <si>
-    <t>::Diagrama de dominio</t>
-  </si>
-  <si>
-    <t>::Diagrama de Estados</t>
-  </si>
-  <si>
     <t>:: Revisão de documentos anteriores (e.g. sistema de avaliação) </t>
   </si>
   <si>
@@ -133,9 +121,6 @@
   </si>
   <si>
     <t>Objetivos de negócio (FEITO)</t>
-  </si>
-  <si>
-    <t>:: requisitos Funcional e Requisitos não funcionais (FEITO)</t>
   </si>
   <si>
     <t>Arquitectura técnica da aplicação (FEITO)</t>
@@ -375,9 +360,6 @@
   </si>
   <si>
     <t>nota minima 10 valores a todas as componentes</t>
-  </si>
-  <si>
-    <t>:: Processo de negócio - BPMN (FEITO)</t>
   </si>
   <si>
     <t>Estudo da Viabilidade(FEITO)</t>
@@ -540,12 +522,33 @@
     <t xml:space="preserve">Fim do Sprint 5
 </t>
   </si>
+  <si>
+    <t>::Diagrama de Estados (FEITO)</t>
+  </si>
+  <si>
+    <t>:: Casos de uso  (JOSE MOURINHO)</t>
+  </si>
+  <si>
+    <t>:: Dossier de organização de grupo (CARLOS)</t>
+  </si>
+  <si>
+    <t>:: Diagrama de modelo de dados (ER) (NÃO FOI PRECISO FAZER)</t>
+  </si>
+  <si>
+    <t>:: Processo de negócio - BPMN (FEITO)</t>
+  </si>
+  <si>
+    <t>:: requisitos Funcional e Requisitos não funcionais (FEITO)</t>
+  </si>
+  <si>
+    <t>::Diagrama de dominio (ENRIQUE)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1276,26 +1279,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6BE823-DED3-4D53-A2A4-88602A1B888D}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="48" workbookViewId="0">
+    <sheetView topLeftCell="C17" zoomScale="48" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="6" width="22.109375" customWidth="1"/>
     <col min="10" max="10" width="19.77734375" customWidth="1"/>
     <col min="14" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.6">
       <c r="A1" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1313,45 +1316,45 @@
       <c r="O2" s="10"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23">
       <c r="A3" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D3" s="53"/>
       <c r="E3" s="52" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F3" s="53"/>
       <c r="G3" s="52" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H3" s="53"/>
       <c r="I3" s="52" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J3" s="53"/>
       <c r="K3" s="52" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L3" s="53"/>
       <c r="M3" s="52" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N3" s="53"/>
       <c r="O3" s="52" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="P3" s="53"/>
     </row>
-    <row r="4" spans="1:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="58.2" customHeight="1">
       <c r="A4" s="50" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
@@ -1378,14 +1381,14 @@
         <v>19</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="O4" s="14">
         <v>20</v>
       </c>
       <c r="P4" s="15"/>
     </row>
-    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.2" customHeight="1">
       <c r="A5" s="51"/>
       <c r="B5" s="33">
         <v>2</v>
@@ -1398,7 +1401,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G5" s="34">
         <v>23</v>
@@ -1416,14 +1419,14 @@
         <v>26</v>
       </c>
       <c r="N5" s="41" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="O5" s="34">
         <v>27</v>
       </c>
       <c r="P5" s="35"/>
     </row>
-    <row r="6" spans="1:23" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="69.599999999999994">
       <c r="A6" s="51"/>
       <c r="B6" s="13">
         <v>3</v>
@@ -1436,7 +1439,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G6" s="14">
         <v>30</v>
@@ -1454,16 +1457,16 @@
         <v>3</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="O6" s="14">
         <v>4</v>
       </c>
       <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="1:23" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="95.4" customHeight="1">
       <c r="A7" s="50" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B7" s="13">
         <v>6</v>
@@ -1476,7 +1479,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G7" s="14">
         <v>7</v>
@@ -1493,14 +1496,14 @@
         <v>10</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="O7" s="14">
         <v>11</v>
       </c>
       <c r="P7" s="15"/>
     </row>
-    <row r="8" spans="1:23" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="113.4" customHeight="1">
       <c r="A8" s="51"/>
       <c r="B8" s="13">
         <v>7</v>
@@ -1513,7 +1516,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G8" s="14">
         <v>14</v>
@@ -1531,14 +1534,14 @@
         <v>17</v>
       </c>
       <c r="N8" s="43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="O8" s="14">
         <v>18</v>
       </c>
       <c r="P8" s="15"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23">
       <c r="A9" s="51"/>
       <c r="B9" s="13">
         <v>8</v>
@@ -1551,7 +1554,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G9" s="14">
         <v>21</v>
@@ -1574,7 +1577,7 @@
       <c r="P9" s="15"/>
       <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:23" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="69.599999999999994">
       <c r="A10" s="51"/>
       <c r="B10" s="13">
         <v>9</v>
@@ -1587,7 +1590,7 @@
         <v>27</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G10" s="14">
         <v>28</v>
@@ -1604,16 +1607,16 @@
         <v>31</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="O10" s="14">
         <v>1</v>
       </c>
       <c r="P10" s="15"/>
     </row>
-    <row r="11" spans="1:23" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="54" customHeight="1">
       <c r="A11" s="50" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B11" s="13">
         <v>10</v>
@@ -1626,7 +1629,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G11" s="14">
         <v>4</v>
@@ -1649,7 +1652,7 @@
       </c>
       <c r="P11" s="15"/>
     </row>
-    <row r="12" spans="1:23" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="57.6" customHeight="1">
       <c r="A12" s="51"/>
       <c r="B12" s="13">
         <v>11</v>
@@ -1678,14 +1681,14 @@
         <v>14</v>
       </c>
       <c r="N12" s="42" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="O12" s="14">
         <v>15</v>
       </c>
       <c r="P12" s="15"/>
     </row>
-    <row r="13" spans="1:23" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="56.4" customHeight="1">
       <c r="A13" s="51"/>
       <c r="B13" s="13">
         <v>12</v>
@@ -1698,7 +1701,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G13" s="14">
         <v>18</v>
@@ -1720,7 +1723,7 @@
       </c>
       <c r="P13" s="15"/>
     </row>
-    <row r="14" spans="1:23" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="67.8" customHeight="1">
       <c r="A14" s="51"/>
       <c r="B14" s="13">
         <v>13</v>
@@ -1749,16 +1752,16 @@
         <v>28</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="O14" s="14">
         <v>29</v>
       </c>
       <c r="P14" s="15"/>
     </row>
-    <row r="15" spans="1:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="34.200000000000003" customHeight="1">
       <c r="A15" s="50" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B15" s="13">
         <v>14</v>
@@ -1771,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G15" s="14">
         <v>2</v>
@@ -1793,7 +1796,7 @@
       </c>
       <c r="P15" s="15"/>
     </row>
-    <row r="16" spans="1:23" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="55.8" customHeight="1">
       <c r="A16" s="51"/>
       <c r="B16" s="13">
         <v>15</v>
@@ -1827,7 +1830,7 @@
       </c>
       <c r="P16" s="15"/>
     </row>
-    <row r="17" spans="1:16" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="52.2" customHeight="1">
       <c r="A17" s="51"/>
       <c r="B17" s="13">
         <v>16</v>
@@ -1840,7 +1843,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="42" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G17" s="14">
         <v>16</v>
@@ -1857,14 +1860,14 @@
         <v>19</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="O17" s="14">
         <v>20</v>
       </c>
       <c r="P17" s="15"/>
     </row>
-    <row r="18" spans="1:16" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="46.8" customHeight="1">
       <c r="A18" s="51"/>
       <c r="B18" s="13">
         <v>17</v>
@@ -1877,7 +1880,7 @@
         <v>22</v>
       </c>
       <c r="F18" s="45" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G18" s="14">
         <v>23</v>
@@ -1900,7 +1903,7 @@
       </c>
       <c r="P18" s="15"/>
     </row>
-    <row r="19" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="51" customHeight="1">
       <c r="A19" s="51"/>
       <c r="B19" s="13">
         <v>18</v>
@@ -1934,9 +1937,9 @@
       </c>
       <c r="P19" s="15"/>
     </row>
-    <row r="20" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="28.8">
       <c r="A20" s="50" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B20" s="13">
         <v>14</v>
@@ -1949,7 +1952,7 @@
         <v>5</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G20" s="14">
         <v>6</v>
@@ -1965,14 +1968,14 @@
         <v>9</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="O20" s="14">
         <v>10</v>
       </c>
       <c r="P20" s="15"/>
     </row>
-    <row r="21" spans="1:16" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="28.2">
       <c r="A21" s="51"/>
       <c r="B21" s="13">
         <v>15</v>
@@ -1993,7 +1996,7 @@
         <v>14</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="19"/>
@@ -2002,7 +2005,7 @@
       <c r="O21" s="14"/>
       <c r="P21" s="15"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16">
       <c r="A22" s="26"/>
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
@@ -2011,7 +2014,7 @@
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16">
       <c r="A23" s="26"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
@@ -2021,17 +2024,17 @@
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16">
       <c r="A24" s="26"/>
       <c r="B24" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="H24" s="27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -2040,17 +2043,17 @@
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16">
       <c r="A25" s="26"/>
       <c r="B25" s="28" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
@@ -2059,17 +2062,17 @@
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16">
       <c r="A26" s="26"/>
       <c r="B26" s="28" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
@@ -2078,43 +2081,43 @@
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16">
       <c r="A27" s="29"/>
       <c r="B27" s="28"/>
       <c r="C27" s="11"/>
       <c r="H27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="29"/>
       <c r="B28" s="30"/>
       <c r="C28" s="11"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16">
       <c r="A29" s="29"/>
       <c r="B29" s="30"/>
       <c r="C29" s="11"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16">
       <c r="A30" s="29"/>
       <c r="B30" s="28"/>
       <c r="C30" s="11"/>
       <c r="H30" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="29"/>
       <c r="B31" s="28"/>
       <c r="C31" s="11"/>
       <c r="H31" s="31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="29"/>
       <c r="B32" s="28"/>
       <c r="C32" s="11"/>
@@ -2122,73 +2125,73 @@
         <v>0.1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" s="29"/>
       <c r="H33" s="32">
         <v>0.25</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" s="29"/>
       <c r="H34" s="32">
         <v>0.25</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35" s="29"/>
       <c r="H35" s="32">
         <v>0.4</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" s="29"/>
       <c r="B36" s="29"/>
       <c r="H36" s="32"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="H37" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
       <c r="H38" s="32"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39" s="29"/>
       <c r="H39" s="32"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" s="29"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41" s="29"/>
     </row>
   </sheetData>
@@ -2221,354 +2224,355 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBF2D1-CADC-44D3-8848-D81CAA5E17FC}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="87" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.6">
       <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.6">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.6">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.6">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15.6">
       <c r="A12" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.6">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.6">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15.6">
       <c r="A15" s="4" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15.6">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.6">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.6">
       <c r="A18" s="1"/>
       <c r="B18" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.6">
       <c r="A19" s="1"/>
       <c r="B19" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.6">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.6">
       <c r="A21" s="1"/>
       <c r="B21" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.6">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.6">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.6">
       <c r="A25" s="4" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.6">
       <c r="A26" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.6">
       <c r="A27" s="4" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.6">
       <c r="A28" s="4" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.6">
       <c r="A29" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.6">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.6">
       <c r="A31" s="1"/>
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.6">
       <c r="A32" s="1"/>
       <c r="B32" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.6">
       <c r="A34" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.6">
       <c r="A35" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.6">
       <c r="A36" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.6">
       <c r="A37" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.6">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="15.6">
       <c r="A39" s="1"/>
       <c r="B39" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.6">
       <c r="A40" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15.6">
       <c r="A41" s="4"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="15.6">
       <c r="A42" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="15.6">
       <c r="A43" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="15.6">
       <c r="A44" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="15.6">
       <c r="A45" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="15.6">
       <c r="A46" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="15.6">
       <c r="A47" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="15.6">
       <c r="A48" s="6"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="15.6">
       <c r="A49" s="4"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="15.6">
       <c r="A50" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="15.6">
       <c r="A51" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="15.6">
       <c r="A52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6">
+      <c r="A53" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="15.6">
       <c r="A54" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="15.6">
       <c r="A55" s="4"/>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="15.6">
       <c r="A56" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="15.6">
       <c r="A58" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="15.6">
       <c r="A59" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="15.6">
       <c r="A60" s="4"/>
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
     </row>

</xml_diff>

<commit_message>
docs: Update Excel & add class diagram image
Updated the excel and added class diagram image for later use in the doc.
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\LojaSocial-IPCA\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\LojaSocial-IPCA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44088F9B-92F4-4867-8AB1-FDA894EDCB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141A7CB4-675D-4033-9259-C03FF34C0115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="2" r:id="rId1"/>
@@ -526,9 +526,6 @@
     <t>::Diagrama de Estados (FEITO)</t>
   </si>
   <si>
-    <t>:: Casos de uso  (JOSE MOURINHO)</t>
-  </si>
-  <si>
     <t>:: Dossier de organização de grupo (CARLOS)</t>
   </si>
   <si>
@@ -541,7 +538,10 @@
     <t>:: requisitos Funcional e Requisitos não funcionais (FEITO)</t>
   </si>
   <si>
-    <t>::Diagrama de dominio (ENRIQUE)</t>
+    <t>::Diagrama de dominio (FEITO)</t>
+  </si>
+  <si>
+    <t>:: Casos de uso  (JOSE)</t>
   </si>
 </sst>
 </file>
@@ -933,17 +933,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hiperligação" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{5250B5AF-2897-4BA3-A5B3-8D8CB871909E}"/>
   </cellStyles>
@@ -961,7 +961,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1283,14 +1283,14 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.6">
+    <row r="1" spans="1:23" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>31</v>
       </c>
@@ -1323,37 +1323,37 @@
       <c r="B3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="52" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="52" t="s">
+      <c r="F3" s="51"/>
+      <c r="G3" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="52" t="s">
+      <c r="H3" s="51"/>
+      <c r="I3" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="52" t="s">
+      <c r="J3" s="51"/>
+      <c r="K3" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="52" t="s">
+      <c r="L3" s="51"/>
+      <c r="M3" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="52" t="s">
+      <c r="N3" s="51"/>
+      <c r="O3" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="53"/>
-    </row>
-    <row r="4" spans="1:23" ht="58.2" customHeight="1">
-      <c r="A4" s="50" t="s">
+      <c r="P3" s="51"/>
+    </row>
+    <row r="4" spans="1:23" ht="58.15" customHeight="1">
+      <c r="A4" s="52" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="13">
@@ -1388,8 +1388,8 @@
       </c>
       <c r="P4" s="15"/>
     </row>
-    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.2" customHeight="1">
-      <c r="A5" s="51"/>
+    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.15" customHeight="1">
+      <c r="A5" s="53"/>
       <c r="B5" s="33">
         <v>2</v>
       </c>
@@ -1426,8 +1426,8 @@
       </c>
       <c r="P5" s="35"/>
     </row>
-    <row r="6" spans="1:23" ht="69.599999999999994">
-      <c r="A6" s="51"/>
+    <row r="6" spans="1:23" ht="73.5">
+      <c r="A6" s="53"/>
       <c r="B6" s="13">
         <v>3</v>
       </c>
@@ -1464,8 +1464,8 @@
       </c>
       <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="1:23" ht="95.4" customHeight="1">
-      <c r="A7" s="50" t="s">
+    <row r="7" spans="1:23" ht="95.45" customHeight="1">
+      <c r="A7" s="52" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="13">
@@ -1503,8 +1503,8 @@
       </c>
       <c r="P7" s="15"/>
     </row>
-    <row r="8" spans="1:23" ht="113.4" customHeight="1">
-      <c r="A8" s="51"/>
+    <row r="8" spans="1:23" ht="113.45" customHeight="1">
+      <c r="A8" s="53"/>
       <c r="B8" s="13">
         <v>7</v>
       </c>
@@ -1541,8 +1541,8 @@
       </c>
       <c r="P8" s="15"/>
     </row>
-    <row r="9" spans="1:23">
-      <c r="A9" s="51"/>
+    <row r="9" spans="1:23" ht="30">
+      <c r="A9" s="53"/>
       <c r="B9" s="13">
         <v>8</v>
       </c>
@@ -1577,8 +1577,8 @@
       <c r="P9" s="15"/>
       <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:23" ht="69.599999999999994">
-      <c r="A10" s="51"/>
+    <row r="10" spans="1:23" ht="73.5">
+      <c r="A10" s="53"/>
       <c r="B10" s="13">
         <v>9</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="P10" s="15"/>
     </row>
     <row r="11" spans="1:23" ht="54" customHeight="1">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="52" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="13">
@@ -1653,7 +1653,7 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:23" ht="57.6" customHeight="1">
-      <c r="A12" s="51"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="13">
         <v>11</v>
       </c>
@@ -1688,8 +1688,8 @@
       </c>
       <c r="P12" s="15"/>
     </row>
-    <row r="13" spans="1:23" ht="56.4" customHeight="1">
-      <c r="A13" s="51"/>
+    <row r="13" spans="1:23" ht="56.45" customHeight="1">
+      <c r="A13" s="53"/>
       <c r="B13" s="13">
         <v>12</v>
       </c>
@@ -1723,8 +1723,8 @@
       </c>
       <c r="P13" s="15"/>
     </row>
-    <row r="14" spans="1:23" ht="67.8" customHeight="1">
-      <c r="A14" s="51"/>
+    <row r="14" spans="1:23" ht="67.900000000000006" customHeight="1">
+      <c r="A14" s="53"/>
       <c r="B14" s="13">
         <v>13</v>
       </c>
@@ -1759,8 +1759,8 @@
       </c>
       <c r="P14" s="15"/>
     </row>
-    <row r="15" spans="1:23" ht="34.200000000000003" customHeight="1">
-      <c r="A15" s="50" t="s">
+    <row r="15" spans="1:23" ht="34.15" customHeight="1">
+      <c r="A15" s="52" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="13">
@@ -1796,8 +1796,8 @@
       </c>
       <c r="P15" s="15"/>
     </row>
-    <row r="16" spans="1:23" ht="55.8" customHeight="1">
-      <c r="A16" s="51"/>
+    <row r="16" spans="1:23" ht="55.9" customHeight="1">
+      <c r="A16" s="53"/>
       <c r="B16" s="13">
         <v>15</v>
       </c>
@@ -1830,8 +1830,8 @@
       </c>
       <c r="P16" s="15"/>
     </row>
-    <row r="17" spans="1:16" ht="52.2" customHeight="1">
-      <c r="A17" s="51"/>
+    <row r="17" spans="1:16" ht="52.15" customHeight="1">
+      <c r="A17" s="53"/>
       <c r="B17" s="13">
         <v>16</v>
       </c>
@@ -1867,8 +1867,8 @@
       </c>
       <c r="P17" s="15"/>
     </row>
-    <row r="18" spans="1:16" ht="46.8" customHeight="1">
-      <c r="A18" s="51"/>
+    <row r="18" spans="1:16" ht="46.9" customHeight="1">
+      <c r="A18" s="53"/>
       <c r="B18" s="13">
         <v>17</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="P18" s="15"/>
     </row>
     <row r="19" spans="1:16" ht="51" customHeight="1">
-      <c r="A19" s="51"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="13">
         <v>18</v>
       </c>
@@ -1937,8 +1937,8 @@
       </c>
       <c r="P19" s="15"/>
     </row>
-    <row r="20" spans="1:16" ht="28.8">
-      <c r="A20" s="50" t="s">
+    <row r="20" spans="1:16" ht="30">
+      <c r="A20" s="52" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="13">
@@ -1975,8 +1975,8 @@
       </c>
       <c r="P20" s="15"/>
     </row>
-    <row r="21" spans="1:16" ht="28.2">
-      <c r="A21" s="51"/>
+    <row r="21" spans="1:16" ht="44.25">
+      <c r="A21" s="53"/>
       <c r="B21" s="13">
         <v>15</v>
       </c>
@@ -2196,6 +2196,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
@@ -2203,11 +2208,6 @@
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F9" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{40893C99-8889-497D-B662-6514644C9EFC}"/>
@@ -2224,11 +2224,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBF2D1-CADC-44D3-8848-D81CAA5E17FC}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="87" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1"/>
@@ -2258,92 +2258,92 @@
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="15.6">
+    <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" ht="15.6">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" ht="15.6">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" ht="15.6">
+    <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="15.6">
+    <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="15.6">
+    <row r="12" spans="1:2" ht="15.75">
       <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="15.6">
+    <row r="13" spans="1:2" ht="15.75">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="15.6">
+    <row r="14" spans="1:2" ht="15.75">
       <c r="A14" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" ht="15.6">
+    <row r="15" spans="1:2" ht="15.75">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="15.6">
+    <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6">
+    <row r="17" spans="1:7" ht="15.75">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6">
+    <row r="18" spans="1:7" ht="15.75">
       <c r="A18" s="1"/>
       <c r="B18" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6">
+    <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="1"/>
       <c r="B19" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.6">
+    <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6">
+    <row r="21" spans="1:7" ht="15.75">
       <c r="A21" s="1"/>
       <c r="B21" s="4" t="s">
         <v>76</v>
@@ -2353,196 +2353,196 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6">
+    <row r="23" spans="1:7" ht="15.75">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6">
+    <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6">
+    <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6">
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6">
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6">
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="1"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6">
+    <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.6">
+    <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="1"/>
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.6">
+    <row r="32" spans="1:7" ht="15.75">
       <c r="A32" s="1"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.6">
+    <row r="33" spans="1:2" ht="15.75">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15.6">
+    <row r="34" spans="1:2" ht="15.75">
       <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" ht="15.6">
+    <row r="35" spans="1:2" ht="15.75">
       <c r="A35" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" ht="15.6">
+    <row r="36" spans="1:2" ht="15.75">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" ht="15.6">
+    <row r="37" spans="1:2" ht="15.75">
       <c r="A37" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" ht="15.6">
+    <row r="38" spans="1:2" ht="15.75">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" ht="15.6">
+    <row r="39" spans="1:2" ht="15.75">
       <c r="A39" s="1"/>
       <c r="B39" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.6">
+    <row r="40" spans="1:2" ht="15.75">
       <c r="A40" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" ht="15.6">
+    <row r="41" spans="1:2" ht="15.75">
       <c r="A41" s="4"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" ht="15.6">
+    <row r="42" spans="1:2" ht="15.75">
       <c r="A42" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:2" ht="15.6">
+    <row r="43" spans="1:2" ht="15.75">
       <c r="A43" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:2" ht="15.6">
+    <row r="44" spans="1:2" ht="15.75">
       <c r="A44" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" ht="15.6">
+    <row r="45" spans="1:2" ht="15.75">
       <c r="A45" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" ht="15.6">
+    <row r="46" spans="1:2" ht="15.75">
       <c r="A46" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" ht="15.6">
+    <row r="47" spans="1:2" ht="15.75">
       <c r="A47" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" ht="15.6">
+    <row r="48" spans="1:2" ht="15.75">
       <c r="A48" s="6"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" ht="15.6">
+    <row r="49" spans="1:2" ht="15.75">
       <c r="A49" s="4"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" ht="15.6">
+    <row r="50" spans="1:2" ht="15.75">
       <c r="A50" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" ht="15.6">
+    <row r="51" spans="1:2" ht="15.75">
       <c r="A51" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" ht="15.6">
+    <row r="52" spans="1:2" ht="15.75">
       <c r="A52" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" ht="15.6">
+    <row r="53" spans="1:2" ht="15.75">
       <c r="A53" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" ht="15.6">
+    <row r="54" spans="1:2" ht="15.75">
       <c r="A54" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" ht="15.6">
+    <row r="55" spans="1:2" ht="15.75">
       <c r="A55" s="4"/>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" ht="15.6">
+    <row r="56" spans="1:2" ht="15.75">
       <c r="A56" s="6" t="s">
         <v>23</v>
       </c>
@@ -2552,19 +2552,19 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" ht="15.6">
+    <row r="58" spans="1:2" ht="15.75">
       <c r="A58" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" ht="15.6">
+    <row r="59" spans="1:2" ht="15.75">
       <c r="A59" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" ht="15.6">
+    <row r="60" spans="1:2" ht="15.75">
       <c r="A60" s="4"/>
       <c r="B60" s="1"/>
     </row>

</xml_diff>

<commit_message>
docs: submission of the second sprint
Submission of the second sprint
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\LojaSocial-IPCA\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Documents\GitHub\LojaSocial-IPCA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141A7CB4-675D-4033-9259-C03FF34C0115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A261A0-109E-4F08-A5AF-075462E9CFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
+    <workbookView xWindow="5676" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{24383FF5-241A-4A8E-A19A-019557CFC8A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="2" r:id="rId1"/>
@@ -526,12 +526,6 @@
     <t>::Diagrama de Estados (FEITO)</t>
   </si>
   <si>
-    <t>:: Dossier de organização de grupo (CARLOS)</t>
-  </si>
-  <si>
-    <t>:: Diagrama de modelo de dados (ER) (NÃO FOI PRECISO FAZER)</t>
-  </si>
-  <si>
     <t>:: Processo de negócio - BPMN (FEITO)</t>
   </si>
   <si>
@@ -541,14 +535,20 @@
     <t>::Diagrama de dominio (FEITO)</t>
   </si>
   <si>
-    <t>:: Casos de uso  (JOSE)</t>
+    <t>:: Dossier de organização de grupo (FEITO)</t>
+  </si>
+  <si>
+    <t>:: Diagrama de modelo de dados (ER) (FEITO)</t>
+  </si>
+  <si>
+    <t>:: Casos de uso  (FEITO)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,6 +676,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri, sans-serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -834,7 +840,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -933,17 +939,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hiperligação" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{5250B5AF-2897-4BA3-A5B3-8D8CB871909E}"/>
   </cellStyles>
@@ -961,7 +968,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1283,14 +1290,14 @@
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75">
+    <row r="1" spans="1:23" ht="15.6">
       <c r="A1" s="8" t="s">
         <v>31</v>
       </c>
@@ -1323,37 +1330,37 @@
       <c r="B3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="50" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="50" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="50" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="51"/>
-      <c r="M3" s="50" t="s">
+      <c r="L3" s="53"/>
+      <c r="M3" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="51"/>
-      <c r="O3" s="50" t="s">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="51"/>
-    </row>
-    <row r="4" spans="1:23" ht="58.15" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="P3" s="53"/>
+    </row>
+    <row r="4" spans="1:23" ht="58.2" customHeight="1">
+      <c r="A4" s="50" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="13">
@@ -1388,8 +1395,8 @@
       </c>
       <c r="P4" s="15"/>
     </row>
-    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.15" customHeight="1">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:23" s="40" customFormat="1" ht="88.2" customHeight="1">
+      <c r="A5" s="51"/>
       <c r="B5" s="33">
         <v>2</v>
       </c>
@@ -1426,8 +1433,8 @@
       </c>
       <c r="P5" s="35"/>
     </row>
-    <row r="6" spans="1:23" ht="73.5">
-      <c r="A6" s="53"/>
+    <row r="6" spans="1:23" ht="69.599999999999994">
+      <c r="A6" s="51"/>
       <c r="B6" s="13">
         <v>3</v>
       </c>
@@ -1464,8 +1471,8 @@
       </c>
       <c r="P6" s="15"/>
     </row>
-    <row r="7" spans="1:23" ht="95.45" customHeight="1">
-      <c r="A7" s="52" t="s">
+    <row r="7" spans="1:23" ht="95.4" customHeight="1">
+      <c r="A7" s="50" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="13">
@@ -1503,8 +1510,8 @@
       </c>
       <c r="P7" s="15"/>
     </row>
-    <row r="8" spans="1:23" ht="113.45" customHeight="1">
-      <c r="A8" s="53"/>
+    <row r="8" spans="1:23" ht="113.4" customHeight="1">
+      <c r="A8" s="51"/>
       <c r="B8" s="13">
         <v>7</v>
       </c>
@@ -1541,8 +1548,8 @@
       </c>
       <c r="P8" s="15"/>
     </row>
-    <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="53"/>
+    <row r="9" spans="1:23">
+      <c r="A9" s="51"/>
       <c r="B9" s="13">
         <v>8</v>
       </c>
@@ -1577,8 +1584,8 @@
       <c r="P9" s="15"/>
       <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:23" ht="73.5">
-      <c r="A10" s="53"/>
+    <row r="10" spans="1:23" ht="69.599999999999994">
+      <c r="A10" s="51"/>
       <c r="B10" s="13">
         <v>9</v>
       </c>
@@ -1615,7 +1622,7 @@
       <c r="P10" s="15"/>
     </row>
     <row r="11" spans="1:23" ht="54" customHeight="1">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="50" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="13">
@@ -1653,7 +1660,7 @@
       <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:23" ht="57.6" customHeight="1">
-      <c r="A12" s="53"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="13">
         <v>11</v>
       </c>
@@ -1688,8 +1695,8 @@
       </c>
       <c r="P12" s="15"/>
     </row>
-    <row r="13" spans="1:23" ht="56.45" customHeight="1">
-      <c r="A13" s="53"/>
+    <row r="13" spans="1:23" ht="56.4" customHeight="1">
+      <c r="A13" s="51"/>
       <c r="B13" s="13">
         <v>12</v>
       </c>
@@ -1723,8 +1730,8 @@
       </c>
       <c r="P13" s="15"/>
     </row>
-    <row r="14" spans="1:23" ht="67.900000000000006" customHeight="1">
-      <c r="A14" s="53"/>
+    <row r="14" spans="1:23" ht="67.95" customHeight="1">
+      <c r="A14" s="51"/>
       <c r="B14" s="13">
         <v>13</v>
       </c>
@@ -1759,8 +1766,8 @@
       </c>
       <c r="P14" s="15"/>
     </row>
-    <row r="15" spans="1:23" ht="34.15" customHeight="1">
-      <c r="A15" s="52" t="s">
+    <row r="15" spans="1:23" ht="34.200000000000003" customHeight="1">
+      <c r="A15" s="50" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="13">
@@ -1796,8 +1803,8 @@
       </c>
       <c r="P15" s="15"/>
     </row>
-    <row r="16" spans="1:23" ht="55.9" customHeight="1">
-      <c r="A16" s="53"/>
+    <row r="16" spans="1:23" ht="55.95" customHeight="1">
+      <c r="A16" s="51"/>
       <c r="B16" s="13">
         <v>15</v>
       </c>
@@ -1830,8 +1837,8 @@
       </c>
       <c r="P16" s="15"/>
     </row>
-    <row r="17" spans="1:16" ht="52.15" customHeight="1">
-      <c r="A17" s="53"/>
+    <row r="17" spans="1:16" ht="52.2" customHeight="1">
+      <c r="A17" s="51"/>
       <c r="B17" s="13">
         <v>16</v>
       </c>
@@ -1867,8 +1874,8 @@
       </c>
       <c r="P17" s="15"/>
     </row>
-    <row r="18" spans="1:16" ht="46.9" customHeight="1">
-      <c r="A18" s="53"/>
+    <row r="18" spans="1:16" ht="46.95" customHeight="1">
+      <c r="A18" s="51"/>
       <c r="B18" s="13">
         <v>17</v>
       </c>
@@ -1904,7 +1911,7 @@
       <c r="P18" s="15"/>
     </row>
     <row r="19" spans="1:16" ht="51" customHeight="1">
-      <c r="A19" s="53"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="13">
         <v>18</v>
       </c>
@@ -1937,8 +1944,8 @@
       </c>
       <c r="P19" s="15"/>
     </row>
-    <row r="20" spans="1:16" ht="30">
-      <c r="A20" s="52" t="s">
+    <row r="20" spans="1:16" ht="28.8">
+      <c r="A20" s="50" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="13">
@@ -1975,8 +1982,8 @@
       </c>
       <c r="P20" s="15"/>
     </row>
-    <row r="21" spans="1:16" ht="44.25">
-      <c r="A21" s="53"/>
+    <row r="21" spans="1:16" ht="28.2">
+      <c r="A21" s="51"/>
       <c r="B21" s="13">
         <v>15</v>
       </c>
@@ -2196,11 +2203,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A10"/>
@@ -2208,6 +2210,11 @@
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F9" location="Entregas!A6" display="1ª Entrega / apresentação" xr:uid="{40893C99-8889-497D-B662-6514644C9EFC}"/>
@@ -2224,11 +2231,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBF2D1-CADC-44D3-8848-D81CAA5E17FC}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1"/>
@@ -2258,92 +2265,92 @@
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75">
+    <row r="8" spans="1:2" ht="15.6">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:2" ht="15.6">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" ht="15.75">
+    <row r="10" spans="1:2" ht="15.6">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" ht="15.75">
+    <row r="11" spans="1:2" ht="15.6">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75">
+    <row r="12" spans="1:2" ht="15.6">
       <c r="A12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
+    <row r="13" spans="1:2" ht="15.6">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
+    <row r="14" spans="1:2" ht="15.6">
       <c r="A14" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
+    <row r="15" spans="1:2" ht="15.6">
       <c r="A15" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75">
+    <row r="16" spans="1:2" ht="15.6">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75">
+    <row r="17" spans="1:7" ht="15.6">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
         <v>73</v>
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75">
+    <row r="18" spans="1:7" ht="15.6">
       <c r="A18" s="1"/>
       <c r="B18" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75">
+    <row r="19" spans="1:7" ht="15.6">
       <c r="A19" s="1"/>
       <c r="B19" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75">
+    <row r="20" spans="1:7" ht="15.6">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75">
+    <row r="21" spans="1:7" ht="15.6">
       <c r="A21" s="1"/>
       <c r="B21" s="4" t="s">
         <v>76</v>
@@ -2353,196 +2360,196 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75">
+    <row r="23" spans="1:7" ht="15.6">
       <c r="A23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75">
+    <row r="24" spans="1:7" ht="15.6">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="15.75">
+    <row r="25" spans="1:7" ht="15.6">
       <c r="A25" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="15.75">
-      <c r="A26" s="4" t="s">
-        <v>94</v>
+    <row r="26" spans="1:7" ht="15.6">
+      <c r="A26" s="54" t="s">
+        <v>97</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75">
+    <row r="27" spans="1:7" ht="15.6">
       <c r="A27" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75">
+    <row r="28" spans="1:7" ht="15.6">
       <c r="A28" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="15.75">
+    <row r="29" spans="1:7" ht="15.6">
       <c r="A29" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B29" s="1"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75">
+    <row r="30" spans="1:7" ht="15.6">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75">
+    <row r="31" spans="1:7" ht="15.6">
       <c r="A31" s="1"/>
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75">
+    <row r="32" spans="1:7" ht="15.6">
       <c r="A32" s="1"/>
       <c r="B32" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75">
+    <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75">
+    <row r="34" spans="1:2" ht="15.6">
       <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75">
+    <row r="35" spans="1:2" ht="15.6">
       <c r="A35" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" ht="15.75">
+    <row r="36" spans="1:2" ht="15.6">
       <c r="A36" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" ht="15.75">
+    <row r="37" spans="1:2" ht="15.6">
       <c r="A37" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" ht="15.75">
+    <row r="38" spans="1:2" ht="15.6">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:2" ht="15.75">
+    <row r="39" spans="1:2" ht="15.6">
       <c r="A39" s="1"/>
       <c r="B39" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15.75">
+    <row r="40" spans="1:2" ht="15.6">
       <c r="A40" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" ht="15.75">
+    <row r="41" spans="1:2" ht="15.6">
       <c r="A41" s="4"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" ht="15.75">
+    <row r="42" spans="1:2" ht="15.6">
       <c r="A42" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:2" ht="15.75">
+    <row r="43" spans="1:2" ht="15.6">
       <c r="A43" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:2" ht="15.75">
+    <row r="44" spans="1:2" ht="15.6">
       <c r="A44" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" ht="15.75">
+    <row r="45" spans="1:2" ht="15.6">
       <c r="A45" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" ht="15.75">
+    <row r="46" spans="1:2" ht="15.6">
       <c r="A46" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" ht="15.75">
+    <row r="47" spans="1:2" ht="15.6">
       <c r="A47" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" ht="15.75">
+    <row r="48" spans="1:2" ht="15.6">
       <c r="A48" s="6"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" ht="15.75">
+    <row r="49" spans="1:2" ht="15.6">
       <c r="A49" s="4"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" ht="15.75">
+    <row r="50" spans="1:2" ht="15.6">
       <c r="A50" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" ht="15.75">
+    <row r="51" spans="1:2" ht="15.6">
       <c r="A51" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" ht="15.75">
+    <row r="52" spans="1:2" ht="15.6">
       <c r="A52" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" ht="15.75">
+    <row r="53" spans="1:2" ht="15.6">
       <c r="A53" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" ht="15.75">
+    <row r="54" spans="1:2" ht="15.6">
       <c r="A54" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" ht="15.75">
+    <row r="55" spans="1:2" ht="15.6">
       <c r="A55" s="4"/>
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" ht="15.75">
+    <row r="56" spans="1:2" ht="15.6">
       <c r="A56" s="6" t="s">
         <v>23</v>
       </c>
@@ -2552,19 +2559,19 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" ht="15.75">
+    <row r="58" spans="1:2" ht="15.6">
       <c r="A58" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" ht="15.75">
+    <row r="59" spans="1:2" ht="15.6">
       <c r="A59" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" ht="15.75">
+    <row r="60" spans="1:2" ht="15.6">
       <c r="A60" s="4"/>
       <c r="B60" s="1"/>
     </row>

</xml_diff>